<commit_message>
Alterando formato de pesquisa
</commit_message>
<xml_diff>
--- a/RPA/IMDb/Filmes.xlsx
+++ b/RPA/IMDb/Filmes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Documents\UiPath\IMDb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\UiPath\2TIAF\RPA\IMDb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55C1590-B2EE-40F7-B500-2114FAC01DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A06049-C20C-4457-BE98-4908708B6232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filmes" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Filmes</t>
-  </si>
-  <si>
-    <t>Ano</t>
   </si>
   <si>
     <t xml:space="preserve">Superman </t>
@@ -104,11 +101,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95C64F7D-6431-4D7C-8963-FCF7C3F3220A}" name="Table1" displayName="Table1" ref="B2:C8" totalsRowShown="0">
-  <autoFilter ref="B2:C8" xr:uid="{95C64F7D-6431-4D7C-8963-FCF7C3F3220A}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95C64F7D-6431-4D7C-8963-FCF7C3F3220A}" name="Table1" displayName="Table1" ref="B2:B8" totalsRowShown="0">
+  <autoFilter ref="B2:B8" xr:uid="{95C64F7D-6431-4D7C-8963-FCF7C3F3220A}"/>
+  <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{71869663-4559-42D4-815D-CD5EED024AB7}" name="Filmes"/>
-    <tableColumn id="2" xr3:uid="{A199836E-C1D0-4384-AF80-307169CD64BF}" name="Ano"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -377,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,60 +384,39 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1987</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>6</v>
-      </c>
-      <c r="C7">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>2012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>